<commit_message>
dbo.xlsx: nueva tabla añadida
</commit_message>
<xml_diff>
--- a/db.xlsx
+++ b/db.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Proyects\htdocs\maileradmin\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2124094C-A278-4F1D-B20A-A17193277B81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5FD1B15-ADE6-4E05-931B-BBB93EB17F16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D007D16D-A70C-4E72-A632-81F6E03833A1}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="25">
   <si>
     <t>id_linea</t>
   </si>
@@ -99,6 +99,18 @@
   </si>
   <si>
     <t>provincia</t>
+  </si>
+  <si>
+    <t>lineas_fuentes_contactos_logs</t>
+  </si>
+  <si>
+    <t>id_linea_fuente_contacto_log</t>
+  </si>
+  <si>
+    <t>accion</t>
+  </si>
+  <si>
+    <t>resultado</t>
   </si>
 </sst>
 </file>
@@ -306,6 +318,117 @@
         <a:xfrm flipH="1">
           <a:off x="9858375" y="1819275"/>
           <a:ext cx="657225" cy="371475"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>333375</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>685800</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7" name="Abrir corchete 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F0D177CC-74FA-F313-D810-C08A2ADA9FC9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6429375" y="2028825"/>
+          <a:ext cx="352425" cy="2105025"/>
+        </a:xfrm>
+        <a:prstGeom prst="leftBracket">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="es-ES" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="9" name="Conector recto de flecha 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{826ADAC1-33C4-A530-B2CB-46748857D997}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6667500" y="4124325"/>
+          <a:ext cx="200025" cy="19050"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -631,10 +754,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1668F4E5-EA72-4019-9D8A-2E69B5AB508E}">
-  <dimension ref="B9:H16"/>
+  <dimension ref="B9:H24"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -742,6 +865,31 @@
         <v>20</v>
       </c>
     </row>
+    <row r="20" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F20" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="21" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F21" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="22" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F22" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F23" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="24" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F24" t="s">
+        <v>24</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
Subida de mi proyecto
</commit_message>
<xml_diff>
--- a/db.xlsx
+++ b/db.xlsx
@@ -1,42 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\practica2\Desktop\Alberto\Ejercicios\maileradmin\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alberto\Desktop\Proyecto\mailer2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92FBF028-CCBC-4556-B78D-0B9CC91D31C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B31E0A9-B396-4085-BF3A-648E0E69A87E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="855" windowWidth="19440" windowHeight="15000" xr2:uid="{D007D16D-A70C-4E72-A632-81F6E03833A1}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{D007D16D-A70C-4E72-A632-81F6E03833A1}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="42">
   <si>
     <t>id_linea</t>
   </si>
@@ -44,9 +33,6 @@
     <t>nombre</t>
   </si>
   <si>
-    <t>url</t>
-  </si>
-  <si>
     <t>imagen</t>
   </si>
   <si>
@@ -77,9 +63,6 @@
     <t>fecha_alta</t>
   </si>
   <si>
-    <t>lineas</t>
-  </si>
-  <si>
     <t>lineas_fuentes</t>
   </si>
   <si>
@@ -126,13 +109,55 @@
   </si>
   <si>
     <t>foto</t>
+  </si>
+  <si>
+    <t>gasolinera</t>
+  </si>
+  <si>
+    <t>C.P.</t>
+  </si>
+  <si>
+    <t>Dirección</t>
+  </si>
+  <si>
+    <t>Horario</t>
+  </si>
+  <si>
+    <t>IDMunicipio</t>
+  </si>
+  <si>
+    <t>Localidad</t>
+  </si>
+  <si>
+    <t>IDProvincia</t>
+  </si>
+  <si>
+    <t>Latitud</t>
+  </si>
+  <si>
+    <t>Longitud</t>
+  </si>
+  <si>
+    <t>Precio Gasoleo A</t>
+  </si>
+  <si>
+    <t>Precio Gasoleo B</t>
+  </si>
+  <si>
+    <t>Precio Gasolina 95 E5</t>
+  </si>
+  <si>
+    <t>Rótulo</t>
+  </si>
+  <si>
+    <t>id-gasolinera</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -147,6 +172,17 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -175,12 +211,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -369,7 +406,7 @@
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>685800</xdr:colOff>
-      <xdr:row>21</xdr:row>
+      <xdr:row>22</xdr:row>
       <xdr:rowOff>133350</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -421,13 +458,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>571500</xdr:colOff>
-      <xdr:row>21</xdr:row>
+      <xdr:row>22</xdr:row>
       <xdr:rowOff>123825</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>21</xdr:row>
+      <xdr:row>22</xdr:row>
       <xdr:rowOff>142875</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -770,176 +807,207 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1668F4E5-EA72-4019-9D8A-2E69B5AB508E}">
-  <dimension ref="B9:H38"/>
+  <dimension ref="B9:H30"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D38" sqref="D38"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="35" customWidth="1"/>
-    <col min="4" max="4" width="33.5703125" customWidth="1"/>
-    <col min="6" max="6" width="44.42578125" customWidth="1"/>
-    <col min="8" max="8" width="46.85546875" customWidth="1"/>
+    <col min="4" max="4" width="33.5546875" customWidth="1"/>
+    <col min="6" max="6" width="44.44140625" customWidth="1"/>
+    <col min="8" max="8" width="46.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B9" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F9" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>15</v>
-      </c>
       <c r="H9" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B10" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D10" t="s">
+        <v>4</v>
+      </c>
+      <c r="F10" t="s">
+        <v>9</v>
+      </c>
+      <c r="H10" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
-        <v>0</v>
-      </c>
-      <c r="D10" t="s">
-        <v>5</v>
-      </c>
-      <c r="F10" t="s">
-        <v>10</v>
-      </c>
-      <c r="H10" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="D11" t="s">
         <v>0</v>
       </c>
       <c r="F11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H11" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
+        <v>30</v>
+      </c>
+      <c r="D12" t="s">
+        <v>5</v>
+      </c>
+      <c r="F12" t="s">
+        <v>8</v>
+      </c>
+      <c r="H12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B13" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B14" t="s">
+        <v>40</v>
+      </c>
+      <c r="D14" t="s">
+        <v>6</v>
+      </c>
+      <c r="F14" t="s">
+        <v>10</v>
+      </c>
+      <c r="H14" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B15" t="s">
+        <v>33</v>
+      </c>
+      <c r="D15" t="s">
         <v>2</v>
       </c>
-      <c r="D12" t="s">
-        <v>6</v>
-      </c>
-      <c r="F12" t="s">
-        <v>9</v>
-      </c>
-      <c r="H12" t="s">
+      <c r="F15" t="s">
+        <v>11</v>
+      </c>
+      <c r="H15" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
+    <row r="16" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B16" t="s">
+        <v>32</v>
+      </c>
+      <c r="D16" t="s">
         <v>3</v>
       </c>
-      <c r="D13" t="s">
-        <v>7</v>
-      </c>
-      <c r="F13" t="s">
-        <v>11</v>
-      </c>
-      <c r="H13" t="s">
+      <c r="H16" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B14" t="s">
+    <row r="17" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B17" t="s">
+        <v>34</v>
+      </c>
+      <c r="H17" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B18" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B19" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B20" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B21" t="s">
+        <v>38</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" ht="15" x14ac:dyDescent="0.35">
+      <c r="B22" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="F22" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B23" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F23" t="s">
         <v>4</v>
       </c>
-      <c r="D14" t="s">
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B24" t="s">
+        <v>24</v>
+      </c>
+      <c r="F24" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B25" t="s">
+        <v>1</v>
+      </c>
+      <c r="F25" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B26" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="27" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B27" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="28" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B28" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="29" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B29" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="30" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B30" t="s">
         <v>3</v>
       </c>
-      <c r="F14" t="s">
-        <v>12</v>
-      </c>
-      <c r="H14" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D15" t="s">
-        <v>4</v>
-      </c>
-      <c r="H15" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="H16" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="F20" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B21" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="F21" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B22" t="s">
-        <v>26</v>
-      </c>
-      <c r="F22" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B23" t="s">
-        <v>1</v>
-      </c>
-      <c r="F23" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B24" t="s">
-        <v>16</v>
-      </c>
-      <c r="F24" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B25" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B26" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B27" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B28" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="38" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D38" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>